<commit_message>
clear changes du to re-opening of files
</commit_message>
<xml_diff>
--- a/arvarto-customer-segmentation/data-dictionary/DIAS Attributes - Values 2017.xlsx
+++ b/arvarto-customer-segmentation/data-dictionary/DIAS Attributes - Values 2017.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\bfernandes\Documents\repositories\portfolio\arvarto-customer-segmentation\data-dictionary\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8CE1305D-86DB-492F-BE80-C5D02D232C72}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{81547BC2-D7CE-4B0F-AC58-AE0AC0B43C87}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-83" yWindow="-83" windowWidth="25966" windowHeight="10366" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="945" yWindow="960" windowWidth="20940" windowHeight="8363" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -4348,8 +4348,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B2:E2260"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A39" workbookViewId="0">
-      <selection activeCell="B39" sqref="B39"/>
+    <sheetView tabSelected="1" topLeftCell="A755" workbookViewId="0">
+      <selection activeCell="E760" sqref="E760"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -28312,9 +28312,12 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance">
-  <documentManagement/>
-</p:properties>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -28367,24 +28370,15 @@
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance">
+  <documentManagement/>
+</p:properties>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{FDBE20A7-1A06-4982-8E6C-B0692E74AD85}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{DE3EA3FA-F7A9-4EB1-BDA9-02346FC3DB01}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -28405,9 +28399,15 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{DE3EA3FA-F7A9-4EB1-BDA9-02346FC3DB01}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{FDBE20A7-1A06-4982-8E6C-B0692E74AD85}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>